<commit_message>
Updating Product and Sprint 3 backlogs
</commit_message>
<xml_diff>
--- a/sprints/Product Backlog.xlsx
+++ b/sprints/Product Backlog.xlsx
@@ -25,43 +25,43 @@
     <t>User</t>
   </si>
   <si>
+    <t>Allow members to browse for items</t>
+  </si>
+  <si>
+    <t>So they can find items they want to borrow</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Allow warehouse to update rental status (Returned, Sent)</t>
+  </si>
+  <si>
+    <t>To assist tracking media</t>
+  </si>
+  <si>
+    <t>Warehouse Employee</t>
+  </si>
+  <si>
+    <t>Allow managers to manage employees (remove and add).</t>
+  </si>
+  <si>
+    <t>So that employees can be hired and fired.</t>
+  </si>
+  <si>
+    <t>Manager Employee</t>
+  </si>
+  <si>
+    <t>Allow warehouse to view outgoing/incoming orders and where to ship to</t>
+  </si>
+  <si>
+    <t>So they can accurately ship the media</t>
+  </si>
+  <si>
     <t>Allow members to register</t>
   </si>
   <si>
     <t>So they can begin using the system</t>
-  </si>
-  <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>Allow members to browse for items</t>
-  </si>
-  <si>
-    <t>So they can find items they want to borrow</t>
-  </si>
-  <si>
-    <t>Allow warehouse to update rental status (Returned, Sent)</t>
-  </si>
-  <si>
-    <t>To assist tracking media</t>
-  </si>
-  <si>
-    <t>Warehouse Employee</t>
-  </si>
-  <si>
-    <t>Allow managers to manage employees (remove and add).</t>
-  </si>
-  <si>
-    <t>So that employees can be hired and fired.</t>
-  </si>
-  <si>
-    <t>Manager Employee</t>
-  </si>
-  <si>
-    <t>Allow warehouse to view outgoing/incoming orders and where to ship to</t>
-  </si>
-  <si>
-    <t>So they can accurately ship the media</t>
   </si>
   <si>
     <t>Allow members to borrow new items (up to 3 at once)</t>
@@ -167,7 +167,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -182,10 +182,6 @@
     <font>
       <sz val="10.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -209,7 +205,7 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -468,7 +464,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>0.0</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -478,7 +474,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -486,32 +482,32 @@
         <v>0.0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -520,7 +516,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -576,7 +572,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -618,7 +614,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -646,7 +642,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -660,7 +656,7 @@
         <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -716,7 +712,7 @@
         <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">

</xml_diff>